<commit_message>
api và update form trạng thái hoạt động khuyến mãi hàng tặng hàng
</commit_message>
<xml_diff>
--- a/public/excel/Donated.xlsx
+++ b/public/excel/Donated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,30 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>10316863</t>
-  </si>
-  <si>
-    <t>TL Vỉ 2 Gôm E-017/FR</t>
-  </si>
-  <si>
-    <t>10315837</t>
-  </si>
-  <si>
-    <t>TL Bộ sáp nặn MCT - C01/DO - 16 món</t>
-  </si>
-  <si>
-    <t>10280962</t>
-  </si>
-  <si>
-    <t>TL Kéo văn phòng SC-016 hộp 20/T240</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Mã SP</t>
   </si>
   <si>
     <t>Tên SP</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Pathways Reading, Writing 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trạng thái </t>
   </si>
 </sst>
 </file>
@@ -389,47 +380,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60015505</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>